<commit_message>
add jannik to fuser contribution
</commit_message>
<xml_diff>
--- a/Contribution_of_Team_Members.xlsx
+++ b/Contribution_of_Team_Members.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d067795\Documents\GitHub\WDIProjekt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jannik\Desktop\WDIProjekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69DA93D-B06F-463F-BD8A-9C402335F2DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F487070-A4C6-4AC5-AA43-9214EE562ED2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{7EF2D3A3-122C-4149-9370-BCDE6AE12154}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7EF2D3A3-122C-4149-9370-BCDE6AE12154}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -197,7 +197,7 @@
     <t>Generate Data Fusers</t>
   </si>
   <si>
-    <t>Carolin, Luka</t>
+    <t>Carolin, Luka, Jannik</t>
   </si>
 </sst>
 </file>
@@ -256,7 +256,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -272,7 +272,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -571,15 +571,15 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="45.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>